<commit_message>
Added new calculations for disk capacity requirements. Also added disk usage as per recommended broker count
</commit_message>
<xml_diff>
--- a/Sizing Calculator.xlsx
+++ b/Sizing Calculator.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishek.walia/Documents/Codes/github/kafka_broker_sizing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B1B49264-D2D2-DB42-A5E6-EE9F3A1AA574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FAD3EF-E738-1246-9831-D97432D59AB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="32760" windowHeight="19600"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="32760" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0" shapeId="0">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>These are recommendations for the number of replica assignment per broker.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R11" authorId="0" shapeId="0">
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -93,10 +106,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">This is the minimum value that should be put everywhere for this property considering your configurations provided above. </t>
-        </r>
-        <r>
-          <rPr>
+          <t xml:space="preserve">This is the total number of replicas per cluster for a steady state of operations. Going more than this number can cause issues in case of controller failures. Please refere here for more details :
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -107,17 +122,61 @@
         </r>
         <r>
           <rPr>
-            <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Putting the property value any less than this would quite possibly error out.</t>
+          <t xml:space="preserve">https://www.confluent.io/blog/apache-kafka-supports-200k-partitions-per-cluster/
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0">
+    <comment ref="R11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This is the minimum value that should be put everywhere for this property considering your configurations provided above. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Putting the property value any less than this would quite possibly error out.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -153,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R12" authorId="0" shapeId="0">
+    <comment ref="R12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -167,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -214,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R13" authorId="0" shapeId="0">
+    <comment ref="R13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -228,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -243,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q14" authorId="0" shapeId="0">
+    <comment ref="Q14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -280,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -295,7 +354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q15" authorId="0" shapeId="0">
+    <comment ref="Q15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -332,121 +391,92 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
+    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
+            <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>These are recommendations for the number of replica assignment per broker.</t>
+          <t xml:space="preserve">You can keep adding more topic details in row 18 thru 28 for various different types of topics.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Remember , its "type" of topics , not every topic. If topics share similar stats, just add the multiplicative factor on Row 27 for that. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Just use the next empty column to add more types of topics in the sheet. Its configured till AZ column to calculate data.
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0">
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">This is the total number of replicas per cluster for a steady state of operations. Going more than this number can cause issues in case of controller failures. Please refere here for more details :
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://www.confluent.io/blog/apache-kafka-supports-200k-partitions-per-cluster/
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+            <color indexed="8"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Partition Count per topic 
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0" shapeId="0">
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">You can keep adding more topic details in row 18 thru 28 for various different types of topics.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Remember , its "type" of topics , not every topic. If topics share similar stats, just add the multiplicative factor on Row 27 for that. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Just use the next empty column to add more types of topics in the sheet. Its configured till AZ column to calculate data.
+            <color indexed="8"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Average message size in Bytes
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -456,42 +486,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Partition Count per topic 
+          <t xml:space="preserve">Number of messages expected for the topic at a cluster level on per second basis
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="8"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Average message size in Bytes
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A23" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="8"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Number of messages expected for the topic at a cluster level on per second basis
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A24" authorId="0" shapeId="0">
+    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -507,7 +507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A25" authorId="0" shapeId="0">
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -522,7 +522,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A26" authorId="0" shapeId="0">
+    <comment ref="A26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -536,7 +536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0">
+    <comment ref="A27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -578,7 +578,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Topic Name</t>
   </si>
@@ -638,9 +638,6 @@
     <t>Topics With Same stats (count)</t>
   </si>
   <si>
-    <t xml:space="preserve">Disk Throughput based broker Count </t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -677,9 +674,6 @@
     <t>Recommended Broker Count</t>
   </si>
   <si>
-    <t>Max Partition Count Per Broker (Equal Distro)</t>
-  </si>
-  <si>
     <t>Max Leader Partitions per Broker</t>
   </si>
   <si>
@@ -704,9 +698,6 @@
     <t xml:space="preserve">Combined N/W traffic based broker count </t>
   </si>
   <si>
-    <t xml:space="preserve">N/W Inbound Traffic based broker Count </t>
-  </si>
-  <si>
     <t>Replication Factor based Broker Count</t>
   </si>
   <si>
@@ -726,12 +717,30 @@
   </si>
   <si>
     <t>Broker Replica Count Soft Limit based broker count</t>
+  </si>
+  <si>
+    <t>Disk Capacity Based broker count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/W Inbound Traffic based broker count </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disk Throughput based broker count </t>
+  </si>
+  <si>
+    <t>Max Partition Count Per Broker</t>
+  </si>
+  <si>
+    <t>Replica Distribution</t>
+  </si>
+  <si>
+    <t>Disk usage per broker (GB)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1018,7 +1027,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1044,181 +1053,113 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1568,11 +1509,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:BA41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1580,6 +1521,8 @@
     <col min="1" max="1" width="44.5" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
     <col min="13" max="13" width="8.83203125" customWidth="1"/>
     <col min="17" max="17" width="8.33203125" customWidth="1"/>
   </cols>
@@ -1596,345 +1539,403 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="46" t="s">
+      <c r="A3" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="48"/>
-      <c r="O3" s="22" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="O3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="24"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="18"/>
     </row>
     <row r="4" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="27"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="21"/>
     </row>
     <row r="5" spans="1:18" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <f>MAX(B6:L6)</f>
-        <v>36</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="30"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="28"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="45"/>
+      <c r="P5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="23"/>
     </row>
     <row r="6" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="str" cm="1">
+      <c r="A6" s="46" t="str" cm="1">
         <f t="array" ref="A6">_xlfn.SWITCH(A5,B6," The Cluster is bound by Average Ingress Network data and considered as minimum, considering Network Ingress throttling for as potential bottleneck for Average data ingress",
 D6," The cluster is limited by Average total bandwidth available for the cluster. Please use the recommended number of brokers to cater well to both Producers and Consumers without bandwidth issues.",
 F6," The cluster is Ingress Disk write bound and the inbound data is more than what the cluster as a whole can handle. Please consider upgrading Disk Write throughput or using the recommended number of brokers",
-H6," The broker count is limited by the replication factor provided in the configuration parameters for the topics.",
-J6," The broker count is limited at the soft limit for replica count per broker node. This is as per recommendations from Jun Rao in his blogs. Please modify cell D16 to taste.")</f>
-        <v xml:space="preserve"> The broker count is limited at the soft limit for replica count per broker node. This is as per recommendations from Jun Rao in his blogs. Please modify cell D16 to taste.</v>
-      </c>
-      <c r="B6" s="31">
+H6," The cluster is disk capacity bound and data retention policy needs either more brokers with equal capacity disks or more disk capacity is needed. This considers equal data distribution across the cluster.",
+J6," The broker count is limited by the replication factor provided in the configuration parameters for the topics.",
+L6," The broker count is limited at the soft limit for replica count per broker node. This is as per recommendations from Jun Rao in his blogs. Please modify cell G11 to taste.")</f>
+        <v xml:space="preserve"> The broker count is limited at the soft limit for replica count per broker node. This is as per recommendations from Jun Rao in his blogs. Please modify cell G11 to taste.</v>
+      </c>
+      <c r="B6" s="29">
         <f>CEILING((L10/D13)/D15,1)</f>
-        <v>3</v>
-      </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="31">
+        <v>2</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="29">
         <f>CEILING(((L12+L10)/(D13+D14))/D15, 1)</f>
+        <v>4</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" s="29">
+        <f>CEILING(((L10+L15)/D11),1)</f>
         <v>7</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="31">
-        <f>CEILING(((L10+L15)/D11),1)</f>
-        <v>10</v>
-      </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="31">
+      <c r="G6" s="30"/>
+      <c r="H6" s="29">
+        <f>CEILING(L14/D10,1)</f>
+        <v>5</v>
+      </c>
+      <c r="I6" s="30"/>
+      <c r="J6" s="29">
         <f>CEILING(B20,1)</f>
         <v>3</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="21">
-        <f>CEILING(L16/D16,1)</f>
-        <v>36</v>
-      </c>
-      <c r="K6" s="21"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="26">
+        <f>CEILING(G12/G10,1)</f>
+        <v>14</v>
+      </c>
+      <c r="M6" s="26"/>
       <c r="O6" s="6"/>
-      <c r="P6" s="44" t="s">
+      <c r="P6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="45"/>
+      <c r="Q6" s="23"/>
     </row>
     <row r="7" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="44" t="s">
+      <c r="P7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="Q7" s="45"/>
+      <c r="Q7" s="23"/>
     </row>
     <row r="8" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="35" t="s">
+      <c r="A8" s="47"/>
+      <c r="B8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="37"/>
-      <c r="H8" s="20" t="s">
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="34"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="43"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="45"/>
     </row>
     <row r="9" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="N9" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="N9" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
       <c r="R9" s="4">
         <f>CEILING(B19/A5,1)</f>
-        <v>57</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="41" t="s">
+      <c r="A10" s="48"/>
+      <c r="B10" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="52">
+      <c r="C10" s="25"/>
+      <c r="D10" s="13">
+        <f>1024</f>
         <v>1024</v>
       </c>
-      <c r="H10" s="13" t="str">
-        <f>A31</f>
+      <c r="E10" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="25"/>
+      <c r="G10" s="15">
+        <v>8000</v>
+      </c>
+      <c r="H10" s="43" t="str">
+        <f t="shared" ref="H10:H16" si="0">A31</f>
         <v>Avg Ingress into Cluster (MBps)</v>
       </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
       <c r="L10" s="4">
-        <f t="shared" ref="L10:L15" si="0">B31</f>
-        <v>776.37</v>
-      </c>
-      <c r="N10" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
+        <f t="shared" ref="L10:L15" si="1">B31</f>
+        <v>704.59</v>
+      </c>
+      <c r="N10" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
       <c r="R10" s="4">
         <f>L17-R9</f>
-        <v>3860</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="52">
-        <v>250</v>
-      </c>
-      <c r="H11" s="13" t="str">
-        <f>A32</f>
+      <c r="B11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="13">
+        <v>350</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="25"/>
+      <c r="G11" s="15">
+        <v>200000</v>
+      </c>
+      <c r="H11" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>Peak Ingress into Cluster (MBps)</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
       <c r="L11" s="4">
-        <f t="shared" si="0"/>
-        <v>3759.77</v>
-      </c>
-      <c r="N11" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="19"/>
+        <f t="shared" si="1"/>
+        <v>3527.84</v>
+      </c>
+      <c r="N11" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="41"/>
       <c r="R11" s="4">
         <f>R14+1024</f>
-        <v>5121024</v>
+        <v>103424</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="53">
+      <c r="B12" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="14">
         <v>0.6</v>
       </c>
-      <c r="H12" s="13" t="str">
-        <f>A33</f>
+      <c r="E12" s="24" t="str">
+        <f>A37</f>
+        <v>Total Partition Count Incl. Replicas</v>
+      </c>
+      <c r="F12" s="25"/>
+      <c r="G12" s="4">
+        <f>$B$37</f>
+        <v>108150</v>
+      </c>
+      <c r="H12" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>Avg Egress from Cluster (MBps)</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
       <c r="L12" s="4">
-        <f t="shared" si="0"/>
-        <v>3662.11</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="19"/>
+        <f t="shared" si="1"/>
+        <v>3518.56</v>
+      </c>
+      <c r="N12" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="41"/>
       <c r="R12" s="4">
         <f>MAX(C22:INDEX(22:22,COLUMNS(22:22)))</f>
-        <v>256000</v>
+        <v>5120</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="52">
-        <v>300</v>
-      </c>
-      <c r="H13" s="13" t="str">
-        <f>A34</f>
+      <c r="B13" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="13">
+        <f>((10*1024)/2)/8</f>
+        <v>640</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="G13" s="4">
+        <f>CEILING(G12/A5,1)</f>
+        <v>7725</v>
+      </c>
+      <c r="H13" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>Peak Egress from Cluster (MBps)</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
       <c r="L13" s="4">
-        <f t="shared" si="0"/>
-        <v>18066.41</v>
-      </c>
-      <c r="N13" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="19"/>
+        <f t="shared" si="1"/>
+        <v>17602.54</v>
+      </c>
+      <c r="N13" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="41"/>
       <c r="R13" s="4">
         <f>R12+1024</f>
-        <v>257024</v>
+        <v>6144</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B14" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="52">
-        <v>400</v>
-      </c>
-      <c r="H14" s="13" t="str">
-        <f>A35</f>
+      <c r="B14" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="13">
+        <f>((10*1024)/2)/8</f>
+        <v>640</v>
+      </c>
+      <c r="H14" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>Overall Disk Capacity required (GB)</v>
       </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
       <c r="L14" s="4">
-        <f t="shared" si="0"/>
-        <v>2057.9299999999998</v>
-      </c>
-      <c r="N14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
+        <f t="shared" si="1"/>
+        <v>4406.1400000000003</v>
+      </c>
+      <c r="N14" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
       <c r="Q14" s="5">
         <v>20</v>
       </c>
       <c r="R14" s="4">
         <f>(MAX(C22:INDEX(22:22,COLUMNS(22:22)))*Q14)</f>
-        <v>5120000</v>
+        <v>102400</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="53">
+      <c r="B15" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="14">
         <v>0.95</v>
       </c>
-      <c r="H15" s="13" t="str">
-        <f>A36</f>
+      <c r="H15" s="43" t="str">
+        <f t="shared" si="0"/>
         <v>Inter broker Replication Bandwidth (MBps)</v>
       </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
       <c r="L15" s="4">
-        <f t="shared" si="0"/>
-        <v>1552.74</v>
-      </c>
-      <c r="N15" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
+        <f t="shared" si="1"/>
+        <v>1409.18</v>
+      </c>
+      <c r="N15" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
       <c r="Q15" s="5">
         <v>10</v>
       </c>
@@ -1944,42 +1945,15 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="54">
-        <v>4000</v>
-      </c>
-      <c r="H16" s="13" t="str">
-        <f>A37</f>
-        <v>Total Partition Count Incl. Replicas</v>
-      </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
+      <c r="H16" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
       <c r="L16" s="4">
-        <f>B37</f>
-        <v>141000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="B17" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="54">
-        <v>200000</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="4">
-        <f>CEILING(L16/A5,1)</f>
-        <v>3917</v>
+        <f>L14/A5</f>
+        <v>314.72428571428571</v>
       </c>
     </row>
     <row r="18" spans="1:53" ht="39" customHeight="1" x14ac:dyDescent="0.2">
@@ -1993,22 +1967,22 @@
         <v>2</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:53" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="10">
         <f>SUM(C19:INDEX(19:19,COLUMNS(19:19)))</f>
-        <v>2025</v>
+        <v>70</v>
       </c>
       <c r="C19" s="12">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D19">
-        <v>2000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:53" ht="17" x14ac:dyDescent="0.2">
@@ -2032,8 +2006,7 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="12">
-        <f>24*7</f>
-        <v>168</v>
+        <v>365</v>
       </c>
       <c r="D21">
         <v>24</v>
@@ -2045,13 +2018,14 @@
       </c>
       <c r="B22" s="10">
         <f>SUM(C22:INDEX(22:22,COLUMNS(22:22)))</f>
-        <v>258048</v>
+        <v>7168</v>
       </c>
       <c r="C22" s="12">
         <v>2048</v>
       </c>
       <c r="D22">
-        <v>256000</v>
+        <f>5*1024</f>
+        <v>5120</v>
       </c>
     </row>
     <row r="23" spans="1:53" ht="17" x14ac:dyDescent="0.2">
@@ -2097,13 +2071,14 @@
       </c>
       <c r="B24" s="10">
         <f>SUM(C24:INDEX(24:24,COLUMNS(24:24)))</f>
-        <v>516096</v>
+        <v>29696</v>
       </c>
       <c r="C24" s="12">
         <v>4096</v>
       </c>
       <c r="D24">
-        <v>512000</v>
+        <f>D22*5</f>
+        <v>25600</v>
       </c>
     </row>
     <row r="25" spans="1:53" ht="17" x14ac:dyDescent="0.2">
@@ -2150,838 +2125,838 @@
     </row>
     <row r="31" spans="1:53" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="3">
         <f>CEILING(SUM(C31:INDEX(31:31,COLUMNS(31:31))),0.01)</f>
-        <v>776.37</v>
+        <v>704.59</v>
       </c>
       <c r="C31">
         <f>((((C22*C23)/1024)/1024)*C27)</f>
         <v>703.125</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:AZ31" si="1">((((D22*D23)/1024)/1024)*D27)</f>
-        <v>73.2421875</v>
+        <f t="shared" ref="D31:AZ31" si="2">((((D22*D23)/1024)/1024)*D27)</f>
+        <v>1.46484375</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AK31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AL31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AN31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AO31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AP31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AQ31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AR31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AS31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AT31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AU31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AV31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AW31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AX31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AY31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AZ31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:53" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" s="3">
         <f>CEILING(SUM(C32:INDEX(32:32,COLUMNS(32:32))),0.01)</f>
-        <v>3759.77</v>
+        <v>3527.84</v>
       </c>
       <c r="C32" s="2">
         <f>((((C24*C25)/1024)/1024)*C27)</f>
         <v>3515.625</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" ref="D32:AZ32" si="2">((((D24*D25)/1024)/1024)*D27)</f>
-        <v>244.140625</v>
+        <f t="shared" ref="D32:AZ32" si="3">((((D24*D25)/1024)/1024)*D27)</f>
+        <v>12.20703125</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AL32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AM32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AN32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AO32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AP32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AQ32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AR32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AS32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AT32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AU32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AV32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AW32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AX32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AY32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AZ32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BA32" s="2"/>
     </row>
     <row r="33" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="3">
         <f>CEILING(SUM(C33:INDEX(33:33,COLUMNS(33:33))),0.01)</f>
-        <v>3662.11</v>
+        <v>3518.56</v>
       </c>
       <c r="C33">
         <f>C31*C26</f>
         <v>3515.625</v>
       </c>
       <c r="D33">
-        <f t="shared" ref="D33:AZ33" si="3">D31*D26</f>
-        <v>146.484375</v>
+        <f t="shared" ref="D33:AZ33" si="4">D31*D26</f>
+        <v>2.9296875</v>
       </c>
       <c r="E33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="X33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AA33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AB33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AC33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AE33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AK33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AL33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AM33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AN33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AO33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AP33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AQ33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AR33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AS33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AT33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AU33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AV33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AW33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AX33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AY33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AZ33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="3">
         <f>CEILING(SUM(C34:INDEX(34:34,COLUMNS(34:34))),0.01)</f>
-        <v>18066.41</v>
+        <v>17602.54</v>
       </c>
       <c r="C34">
         <f>C32*C26</f>
         <v>17578.125</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:AZ34" si="4">D32*D26</f>
-        <v>488.28125</v>
+        <f t="shared" ref="D34:AZ34" si="5">D32*D26</f>
+        <v>24.4140625</v>
       </c>
       <c r="E34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AD34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AF34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AG34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AH34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AI34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AJ34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AK34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AL34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AM34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AN34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AO34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AP34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AQ34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AR34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AS34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AT34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AU34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AV34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AW34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AX34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AY34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AZ34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2991,650 +2966,636 @@
       </c>
       <c r="B35" s="3">
         <f>CEILING((SUM(C35:INDEX(35:35,COLUMNS(35:35))))/D12,0.01)</f>
-        <v>2057.9299999999998</v>
+        <v>4406.1400000000003</v>
       </c>
       <c r="C35">
         <f>(((C31*C21*60*60*C20)/1024)/1024)</f>
-        <v>1216.6500091552734</v>
+        <v>2643.3169841766357</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:AZ35" si="5">(((D31*D21*60*60*D20)/1024)/1024)</f>
-        <v>18.104910850524902</v>
+        <f t="shared" ref="D35:AZ35" si="6">(((D31*D21*60*60*D20)/1024)/1024)</f>
+        <v>0.36209821701049805</v>
       </c>
       <c r="E35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Z35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AH35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AJ35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AK35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AL35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AM35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AN35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AO35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AP35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AQ35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AR35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AS35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AT35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AU35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AV35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AW35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AX35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AY35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AZ35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="3">
         <f>CEILING(SUM(C36:INDEX(36:36,COLUMNS(36:36))),0.01)</f>
-        <v>1552.74</v>
+        <v>1409.18</v>
       </c>
       <c r="C36">
         <f>C31*(C20-1)</f>
         <v>1406.25</v>
       </c>
       <c r="D36">
-        <f t="shared" ref="D36:AZ36" si="6">D31*(D20-1)</f>
-        <v>146.484375</v>
+        <f t="shared" ref="D36:AZ36" si="7">D31*(D20-1)</f>
+        <v>2.9296875</v>
       </c>
       <c r="E36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="T36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="U36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AA36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AE36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AH36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AI36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AK36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AL36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AM36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AN36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AO36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AP36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AQ36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AR36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AS36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AT36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AU36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AV36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AW36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AX36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AY36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AZ36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" s="3">
         <f>CEILING(SUM(C37:INDEX(37:37,COLUMNS(37:37))),0.01)</f>
-        <v>141000</v>
+        <v>108150</v>
       </c>
       <c r="C37">
         <f>C27*C19*C20</f>
-        <v>135000</v>
+        <v>108000</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:AZ37" si="7">D27*D19*D20</f>
-        <v>6000</v>
+        <f t="shared" ref="D37:AZ37" si="8">D27*D19*D20</f>
+        <v>150</v>
       </c>
       <c r="E37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="S37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AB37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AJ37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AK37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AL37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AM37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AN37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AO37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AP37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AQ37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AR37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AS37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AT37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AU37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AV37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AW37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AX37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AY37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AZ37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <mergeCells count="42">
-    <mergeCell ref="O3:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="B3:K4"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="J6:K7"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G7"/>
+  <mergeCells count="46">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E8:G9"/>
+    <mergeCell ref="B3:M4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I7"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="N12:Q12"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="B5:C5"/>
@@ -3646,27 +3607,44 @@
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="H8:L9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="P6:Q6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E7"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="P6:Q6"/>
     <mergeCell ref="N9:Q9"/>
     <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="A6:A10"/>
     <mergeCell ref="N13:Q13"/>
     <mergeCell ref="N14:P14"/>
     <mergeCell ref="N15:P15"/>
   </mergeCells>
-  <conditionalFormatting sqref="L16">
-    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="greaterThan">
-      <formula>$D$17</formula>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">
+      <formula>$G$11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L17">
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThan">
-      <formula>$D$16</formula>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="greaterThan">
+      <formula>$G$11</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed Size Requirement calculation and added approximate Leader Follower count per broker
</commit_message>
<xml_diff>
--- a/Sizing Calculator.xlsx
+++ b/Sizing Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishek.walia/Documents/Codes/github/kafka_broker_sizing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FAD3EF-E738-1246-9831-D97432D59AB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7687E2E5-71AE-9044-9D94-222FE5814709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="32760" windowHeight="19600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -270,20 +270,6 @@
           </rPr>
           <t xml:space="preserve">
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="8"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">This value is recommended on the broker side to prevent any errors at broker side due to message size </t>
         </r>
       </text>
     </comment>
@@ -674,12 +660,6 @@
     <t>Recommended Broker Count</t>
   </si>
   <si>
-    <t>Max Leader Partitions per Broker</t>
-  </si>
-  <si>
-    <t>Max Fetcher Partitions per Broker</t>
-  </si>
-  <si>
     <t>batch.size</t>
   </si>
   <si>
@@ -692,9 +672,6 @@
     <t>message.max.bytes</t>
   </si>
   <si>
-    <t>buffer.memory</t>
-  </si>
-  <si>
     <t xml:space="preserve">Combined N/W traffic based broker count </t>
   </si>
   <si>
@@ -735,13 +712,22 @@
   </si>
   <si>
     <t>Disk usage per broker (GB)</t>
+  </si>
+  <si>
+    <t>Leader Partition Count</t>
+  </si>
+  <si>
+    <t>Approximate Leader Partitions per Broker</t>
+  </si>
+  <si>
+    <t>Approximate Fetcher Partitions per Broker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -754,13 +740,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -855,7 +834,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1007,18 +986,284 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1027,12 +1272,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1045,9 +1290,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1056,22 +1298,46 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1081,51 +1347,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1134,52 +1355,90 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1513,7 +1772,7 @@
   <dimension ref="A2:BA41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1527,7 +1786,7 @@
     <col min="17" max="17" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1539,84 +1798,84 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="O3" s="16" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="46"/>
+      <c r="O3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="18"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="25"/>
     </row>
-    <row r="4" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="21"/>
+    <row r="4" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="57"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="28"/>
     </row>
     <row r="5" spans="1:18" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9">
+      <c r="A5" s="37">
         <f>MAX(B6:L6)</f>
-        <v>14</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="54"/>
+      <c r="F5" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="28"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="54"/>
+      <c r="J5" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="54"/>
+      <c r="L5" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="54"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="22" t="s">
+      <c r="P5" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="23"/>
+      <c r="Q5" s="30"/>
     </row>
     <row r="6" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="str" cm="1">
+      <c r="A6" s="38" t="str" cm="1">
         <f t="array" ref="A6">_xlfn.SWITCH(A5,B6," The Cluster is bound by Average Ingress Network data and considered as minimum, considering Network Ingress throttling for as potential bottleneck for Average data ingress",
 D6," The cluster is limited by Average total bandwidth available for the cluster. Please use the recommended number of brokers to cater well to both Producers and Consumers without bandwidth issues.",
 F6," The cluster is Ingress Disk write bound and the inbound data is more than what the cluster as a whole can handle. Please consider upgrading Disk Write throughput or using the recommended number of brokers",
@@ -1625,335 +1884,331 @@
 L6," The broker count is limited at the soft limit for replica count per broker node. This is as per recommendations from Jun Rao in his blogs. Please modify cell G11 to taste.")</f>
         <v xml:space="preserve"> The broker count is limited at the soft limit for replica count per broker node. This is as per recommendations from Jun Rao in his blogs. Please modify cell G11 to taste.</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="47">
         <f>CEILING((L10/D13)/D15,1)</f>
-        <v>2</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="29">
+        <v>1</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="47">
         <f>CEILING(((L12+L10)/(D13+D14))/D15, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="55"/>
+      <c r="F6" s="47">
+        <f>CEILING(((L10+L15)/D11),1)</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="55"/>
+      <c r="H6" s="47">
+        <f>CEILING(L14/D10,1)</f>
+        <v>8</v>
+      </c>
+      <c r="I6" s="55"/>
+      <c r="J6" s="47">
+        <f>CEILING(B20,1)</f>
         <v>4</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="29">
-        <f>CEILING(((L10+L15)/D11),1)</f>
+      <c r="K6" s="55"/>
+      <c r="L6" s="58">
+        <f>CEILING(G12/G10,1)</f>
+        <v>9</v>
+      </c>
+      <c r="M6" s="48"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="29">
-        <f>CEILING(L14/D10,1)</f>
-        <v>5</v>
-      </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="29">
-        <f>CEILING(B20,1)</f>
-        <v>3</v>
-      </c>
-      <c r="K6" s="30"/>
-      <c r="L6" s="26">
-        <f>CEILING(G12/G10,1)</f>
-        <v>14</v>
-      </c>
-      <c r="M6" s="26"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q6" s="23"/>
+      <c r="Q6" s="30"/>
     </row>
-    <row r="7" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="47"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
+    <row r="7" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="50"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="22" t="s">
+      <c r="P7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="Q7" s="23"/>
+      <c r="Q7" s="30"/>
     </row>
     <row r="8" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="47"/>
-      <c r="B8" s="33" t="s">
+      <c r="A8" s="39"/>
+      <c r="B8" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="44" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="41"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="45"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="R8" s="60"/>
     </row>
     <row r="9" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="N9" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="43"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="N9" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
       <c r="R9" s="4">
-        <f>CEILING(B19/A5,1)</f>
-        <v>5</v>
+        <f>CEILING(B38/L6,1)</f>
+        <v>1117</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48"/>
-      <c r="B10" s="24" t="s">
+    <row r="10" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
+      <c r="B10" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="13">
-        <f>1024</f>
-        <v>1024</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="15">
-        <v>8000</v>
-      </c>
-      <c r="H10" s="43" t="str">
-        <f t="shared" ref="H10:H16" si="0">A31</f>
+      <c r="C10" s="16"/>
+      <c r="D10" s="12">
+        <f>1024*4</f>
+        <v>4096</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="14">
+        <v>4500</v>
+      </c>
+      <c r="H10" s="20" t="str">
+        <f t="shared" ref="H10:H15" si="0">A31</f>
         <v>Avg Ingress into Cluster (MBps)</v>
       </c>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="4">
         <f t="shared" ref="L10:L15" si="1">B31</f>
-        <v>704.59</v>
-      </c>
-      <c r="N10" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="43"/>
+        <v>196.78</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
       <c r="R10" s="4">
-        <f>L17-R9</f>
-        <v>-5</v>
+        <f>CEILING(G13-R9, 1)</f>
+        <v>3345</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="13">
+      <c r="C11" s="16"/>
+      <c r="D11" s="12">
         <v>350</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="15">
-        <v>200000</v>
-      </c>
-      <c r="H11" s="43" t="str">
+      <c r="E11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="14">
+        <v>120000</v>
+      </c>
+      <c r="H11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Peak Ingress into Cluster (MBps)</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>3527.84</v>
-      </c>
-      <c r="N11" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="41"/>
+        <v>988.77</v>
+      </c>
+      <c r="N11" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="33"/>
       <c r="R11" s="4">
         <f>R14+1024</f>
-        <v>103424</v>
+        <v>257024</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="14">
-        <v>0.6</v>
-      </c>
-      <c r="E12" s="24" t="str">
+      <c r="B12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="E12" s="15" t="str">
         <f>A37</f>
         <v>Total Partition Count Incl. Replicas</v>
       </c>
-      <c r="F12" s="25"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="4">
         <f>$B$37</f>
-        <v>108150</v>
-      </c>
-      <c r="H12" s="43" t="str">
+        <v>40150</v>
+      </c>
+      <c r="H12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Avg Egress from Cluster (MBps)</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>3518.56</v>
-      </c>
-      <c r="N12" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="41"/>
+        <v>979.5</v>
+      </c>
+      <c r="N12" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="33"/>
       <c r="R12" s="4">
-        <f>MAX(C22:INDEX(22:22,COLUMNS(22:22)))</f>
-        <v>5120</v>
+        <f>MAX(C24:INDEX(24:24,COLUMNS(24:24)))+1024</f>
+        <v>26624</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="13">
+      <c r="C13" s="16"/>
+      <c r="D13" s="12">
         <f>((10*1024)/2)/8</f>
         <v>640</v>
       </c>
-      <c r="E13" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="25"/>
+      <c r="E13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="16"/>
       <c r="G13" s="4">
         <f>CEILING(G12/A5,1)</f>
-        <v>7725</v>
-      </c>
-      <c r="H13" s="43" t="str">
+        <v>4462</v>
+      </c>
+      <c r="H13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Peak Egress from Cluster (MBps)</v>
       </c>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>17602.54</v>
-      </c>
-      <c r="N13" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="4">
-        <f>R12+1024</f>
-        <v>6144</v>
-      </c>
+        <v>4907.2300000000005</v>
+      </c>
+      <c r="N13" s="31"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B14" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="13">
+      <c r="B14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="12">
         <f>((10*1024)/2)/8</f>
         <v>640</v>
       </c>
-      <c r="H14" s="43" t="str">
+      <c r="H14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Overall Disk Capacity required (GB)</v>
       </c>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
       <c r="L14" s="4">
         <f t="shared" si="1"/>
-        <v>4406.1400000000003</v>
-      </c>
-      <c r="N14" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="O14" s="43"/>
-      <c r="P14" s="43"/>
+        <v>31919.21</v>
+      </c>
+      <c r="N14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
       <c r="Q14" s="5">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="R14" s="4">
         <f>(MAX(C22:INDEX(22:22,COLUMNS(22:22)))*Q14)</f>
-        <v>102400</v>
+        <v>256000</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="14">
+      <c r="B15" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="13">
         <v>0.95</v>
       </c>
-      <c r="H15" s="43" t="str">
+      <c r="H15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Inter broker Replication Bandwidth (MBps)</v>
       </c>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
-        <v>1409.18</v>
-      </c>
-      <c r="N15" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
+        <v>588.87</v>
+      </c>
+      <c r="N15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
       <c r="Q15" s="5">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="R15" s="4">
         <f>(1000/(MIN(C23:INDEX(23:23,COLUMNS(23:23)))))*Q15</f>
-        <v>50</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="H16" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
+      <c r="H16" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="4">
         <f>L14/A5</f>
-        <v>314.72428571428571</v>
+        <v>3546.5788888888887</v>
       </c>
     </row>
     <row r="18" spans="1:53" ht="39" customHeight="1" x14ac:dyDescent="0.2">
@@ -1963,7 +2218,7 @@
       <c r="B18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -1974,11 +2229,11 @@
       <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <f>SUM(C19:INDEX(19:19,COLUMNS(19:19)))</f>
         <v>70</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>20</v>
       </c>
       <c r="D19">
@@ -1989,12 +2244,12 @@
       <c r="A20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <f>MAX(C20:AZ20)</f>
-        <v>3</v>
-      </c>
-      <c r="C20" s="12">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C20" s="11">
+        <v>4</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -2004,9 +2259,9 @@
       <c r="A21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="12">
-        <v>365</v>
+      <c r="B21" s="9"/>
+      <c r="C21" s="11">
+        <v>8</v>
       </c>
       <c r="D21">
         <v>24</v>
@@ -2016,11 +2271,11 @@
       <c r="A22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <f>SUM(C22:INDEX(22:22,COLUMNS(22:22)))</f>
         <v>7168</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <v>2048</v>
       </c>
       <c r="D22">
@@ -2032,11 +2287,11 @@
       <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <f>SUM(C23:INDEX(23:23,COLUMNS(23:23)))</f>
         <v>500</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <v>200</v>
       </c>
       <c r="D23" s="2">
@@ -2069,11 +2324,11 @@
       <c r="A24" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <f>SUM(C24:INDEX(24:24,COLUMNS(24:24)))</f>
         <v>29696</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="11">
         <v>4096</v>
       </c>
       <c r="D24">
@@ -2085,11 +2340,11 @@
       <c r="A25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <f>SUM(C25:INDEX(25:25,COLUMNS(25:25)))</f>
         <v>1000</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="11">
         <v>500</v>
       </c>
       <c r="D25" s="2">
@@ -2100,8 +2355,8 @@
       <c r="A26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="12">
+      <c r="B26" s="9"/>
+      <c r="C26" s="11">
         <v>5</v>
       </c>
       <c r="D26">
@@ -2112,12 +2367,12 @@
       <c r="A27" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="9">
         <f>SUM(C27:INDEX(27:27,COLUMNS(27:27)))</f>
-        <v>1801</v>
-      </c>
-      <c r="C27" s="12">
-        <v>1800</v>
+        <v>501</v>
+      </c>
+      <c r="C27" s="11">
+        <v>500</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
@@ -2129,11 +2384,11 @@
       </c>
       <c r="B31" s="3">
         <f>CEILING(SUM(C31:INDEX(31:31,COLUMNS(31:31))),0.01)</f>
-        <v>704.59</v>
+        <v>196.78</v>
       </c>
       <c r="C31">
         <f>((((C22*C23)/1024)/1024)*C27)</f>
-        <v>703.125</v>
+        <v>195.3125</v>
       </c>
       <c r="D31">
         <f t="shared" ref="D31:AZ31" si="2">((((D22*D23)/1024)/1024)*D27)</f>
@@ -2338,11 +2593,11 @@
       </c>
       <c r="B32" s="3">
         <f>CEILING(SUM(C32:INDEX(32:32,COLUMNS(32:32))),0.01)</f>
-        <v>3527.84</v>
+        <v>988.77</v>
       </c>
       <c r="C32" s="2">
         <f>((((C24*C25)/1024)/1024)*C27)</f>
-        <v>3515.625</v>
+        <v>976.5625</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" ref="D32:AZ32" si="3">((((D24*D25)/1024)/1024)*D27)</f>
@@ -2548,11 +2803,11 @@
       </c>
       <c r="B33" s="3">
         <f>CEILING(SUM(C33:INDEX(33:33,COLUMNS(33:33))),0.01)</f>
-        <v>3518.56</v>
+        <v>979.5</v>
       </c>
       <c r="C33">
         <f>C31*C26</f>
-        <v>3515.625</v>
+        <v>976.5625</v>
       </c>
       <c r="D33">
         <f t="shared" ref="D33:AZ33" si="4">D31*D26</f>
@@ -2757,11 +3012,11 @@
       </c>
       <c r="B34" s="3">
         <f>CEILING(SUM(C34:INDEX(34:34,COLUMNS(34:34))),0.01)</f>
-        <v>17602.54</v>
+        <v>4907.2300000000005</v>
       </c>
       <c r="C34">
         <f>C32*C26</f>
-        <v>17578.125</v>
+        <v>4882.8125</v>
       </c>
       <c r="D34">
         <f t="shared" ref="D34:AZ34" si="5">D32*D26</f>
@@ -2966,15 +3221,15 @@
       </c>
       <c r="B35" s="3">
         <f>CEILING((SUM(C35:INDEX(35:35,COLUMNS(35:35))))/D12,0.01)</f>
-        <v>4406.1400000000003</v>
+        <v>31919.21</v>
       </c>
       <c r="C35">
-        <f>(((C31*C21*60*60*C20)/1024)/1024)</f>
-        <v>2643.3169841766357</v>
+        <f>((C31*C21*60*60*C20)/1024)</f>
+        <v>21972.65625</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:AZ35" si="6">(((D31*D21*60*60*D20)/1024)/1024)</f>
-        <v>0.36209821701049805</v>
+        <f t="shared" ref="D35:AZ35" si="6">((D31*D21*60*60*D20)/1024)</f>
+        <v>370.78857421875</v>
       </c>
       <c r="E35">
         <f t="shared" si="6"/>
@@ -3175,11 +3430,11 @@
       </c>
       <c r="B36" s="3">
         <f>CEILING(SUM(C36:INDEX(36:36,COLUMNS(36:36))),0.01)</f>
-        <v>1409.18</v>
+        <v>588.87</v>
       </c>
       <c r="C36">
         <f>C31*(C20-1)</f>
-        <v>1406.25</v>
+        <v>585.9375</v>
       </c>
       <c r="D36">
         <f t="shared" ref="D36:AZ36" si="7">D31*(D20-1)</f>
@@ -3384,11 +3639,11 @@
       </c>
       <c r="B37" s="3">
         <f>CEILING(SUM(C37:INDEX(37:37,COLUMNS(37:37))),0.01)</f>
-        <v>108150</v>
+        <v>40150</v>
       </c>
       <c r="C37">
         <f>C27*C19*C20</f>
-        <v>108000</v>
+        <v>40000</v>
       </c>
       <c r="D37">
         <f t="shared" ref="D37:AZ37" si="8">D27*D19*D20</f>
@@ -3584,18 +3839,241 @@
       </c>
       <c r="AZ37">
         <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="3">
+        <f>CEILING(SUM(C38:INDEX(38:38,COLUMNS(38:38))),0.01)</f>
+        <v>10050</v>
+      </c>
+      <c r="C38">
+        <f>C19*C27</f>
+        <v>10000</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ref="D38:AZ38" si="9">D19*D27</f>
+        <v>50</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AC38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AG38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AH38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AI38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AJ38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AL38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AM38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AN38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AO38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AP38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AQ38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AR38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AS38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AT38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AU38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AV38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AW38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AX38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AY38">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AZ38">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:52" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E8:G9"/>
-    <mergeCell ref="B3:M4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="J6:K7"/>
+    <mergeCell ref="B8:D9"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="B5:C5"/>
@@ -3612,30 +4090,16 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="A6:A10"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E8:G9"/>
+    <mergeCell ref="B3:M4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I7"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="L6:M7"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="J6:K7"/>
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="O3:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="N10:Q10"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="N15:P15"/>
   </mergeCells>
   <conditionalFormatting sqref="G12">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">

</xml_diff>

<commit_message>
Corrected some hard coding in stage 2
</commit_message>
<xml_diff>
--- a/Sizing Calculator.xlsx
+++ b/Sizing Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishek.walia/Documents/Codes/github/kafka_broker_sizing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB448FD-0D0F-4343-B101-4CB6429200AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC7E905-5B9E-0243-B994-5A69C286571E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="38400" windowHeight="22640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2600" yWindow="-26560" windowWidth="38400" windowHeight="22640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage 1" sheetId="2" r:id="rId1"/>
@@ -548,7 +548,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="8"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -584,7 +584,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
   <si>
     <t>Topic Name</t>
   </si>
@@ -746,40 +746,19 @@
     <t>BUName</t>
   </si>
   <si>
-    <t>objectType</t>
-  </si>
-  <si>
-    <t>attrN*</t>
-  </si>
-  <si>
     <t>Version</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>dev</t>
-  </si>
-  <si>
     <t>v1</t>
-  </si>
-  <si>
-    <t>Storage Requirement (GB)</t>
-  </si>
-  <si>
-    <t>Ingress Throughput (MBps)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Egress Throughput (MBps) </t>
   </si>
   <si>
     <t xml:space="preserve">Partition count is your currency, don’t waste it ! </t>
   </si>
   <si>
     <t>Total Partitions in the cluster</t>
-  </si>
-  <si>
-    <t>Minimum partition Count</t>
   </si>
   <si>
     <t>Maximum limit on per Partition Ingress (KBps)</t>
@@ -833,31 +812,55 @@
     <t>Sr No</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>object</t>
-  </si>
-  <si>
-    <t>obj2</t>
-  </si>
-  <si>
     <t>Slowest Consumer Speed (message count/sec/ConsumerInstance )</t>
   </si>
   <si>
-    <t>uat</t>
+    <t>Partition Count Per Topic</t>
   </si>
   <si>
-    <t>test3</t>
+    <t>appName</t>
   </si>
   <si>
-    <t>dataplane</t>
+    <t>ObjName</t>
   </si>
   <si>
-    <t>datanode</t>
+    <t>addlAttr*</t>
   </si>
   <si>
-    <t>Partition Count Per Topic</t>
+    <t>DC/Location</t>
+  </si>
+  <si>
+    <t>prod</t>
+  </si>
+  <si>
+    <t>ordering</t>
+  </si>
+  <si>
+    <t>Storage Requirement - Uncompressed (GB)</t>
+  </si>
+  <si>
+    <t>Ingress Throughput - Buffered (MBps)</t>
+  </si>
+  <si>
+    <t>Egress Throughput (MBps)</t>
+  </si>
+  <si>
+    <t>Minimum partition Count (Default Value)</t>
+  </si>
+  <si>
+    <t>streamdata</t>
+  </si>
+  <si>
+    <t>useast</t>
+  </si>
+  <si>
+    <t>oredering</t>
+  </si>
+  <si>
+    <t>soak</t>
+  </si>
+  <si>
+    <t>uswest</t>
   </si>
 </sst>
 </file>
@@ -1668,11 +1671,50 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1685,21 +1727,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1764,38 +1791,14 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1836,10 +1839,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2142,7 +2141,7 @@
   <dimension ref="A1:K997"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2164,31 +2163,35 @@
     </row>
     <row r="2" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B2" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="D2" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="E2" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="J2" t="str">
+        <f>_xlfn.TEXTJOIN($J$1,TRUE,C2:H2)</f>
+        <v>ENV.BUName.appName.ObjName.addlAttr*.Version</v>
+      </c>
+      <c r="K2" t="s">
         <v>54</v>
-      </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" t="str">
-        <f>_xlfn.TEXTJOIN($J$1,TRUE,B2:H2)</f>
-        <v>ENV.BUName.objectType.attrN*.Version</v>
-      </c>
-      <c r="K2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2196,26 +2199,23 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
         <v>82</v>
       </c>
-      <c r="D4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" t="s">
-        <v>84</v>
-      </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" ref="J4:J35" si="0">_xlfn.TEXTJOIN($J$1,TRUE,B4:H4)</f>
-        <v>dev.test.test.object.obj2.v1</v>
+        <f>_xlfn.TEXTJOIN($J$1,TRUE,$B4:$H4)</f>
+        <v>useast.prod.streamdata.ordering.v1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2223,26 +2223,23 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
         <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" t="s">
         <v>89</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>uat.test.test3.dataplane.datanode.v1</v>
+        <f t="shared" ref="J5:J68" si="0">_xlfn.TEXTJOIN($J$1,TRUE,$B5:$H5)</f>
+        <v>uswest.soak.streamdata.oredering.v1</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2536,7 +2533,7 @@
         <v>33</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" ref="J36:J65" si="1">_xlfn.TEXTJOIN($J$1,TRUE,B36:H36)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2545,7 +2542,7 @@
         <v>34</v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2554,7 +2551,7 @@
         <v>35</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2563,7 +2560,7 @@
         <v>36</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2572,7 +2569,7 @@
         <v>37</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2581,7 +2578,7 @@
         <v>38</v>
       </c>
       <c r="J41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2590,7 +2587,7 @@
         <v>39</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2599,7 +2596,7 @@
         <v>40</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2608,7 +2605,7 @@
         <v>41</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2617,7 +2614,7 @@
         <v>42</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2626,7 +2623,7 @@
         <v>43</v>
       </c>
       <c r="J46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2635,7 +2632,7 @@
         <v>44</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2644,7 +2641,7 @@
         <v>45</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2653,7 +2650,7 @@
         <v>46</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2662,7 +2659,7 @@
         <v>47</v>
       </c>
       <c r="J50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2671,7 +2668,7 @@
         <v>48</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2680,7 +2677,7 @@
         <v>49</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2689,7 +2686,7 @@
         <v>50</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2698,7 +2695,7 @@
         <v>51</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2707,7 +2704,7 @@
         <v>52</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2716,7 +2713,7 @@
         <v>53</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2725,7 +2722,7 @@
         <v>54</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2734,7 +2731,7 @@
         <v>55</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2743,7 +2740,7 @@
         <v>56</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2752,7 +2749,7 @@
         <v>57</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2761,7 +2758,7 @@
         <v>58</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2770,7 +2767,7 @@
         <v>59</v>
       </c>
       <c r="J62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2779,7 +2776,7 @@
         <v>60</v>
       </c>
       <c r="J63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2788,7 +2785,7 @@
         <v>61</v>
       </c>
       <c r="J64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2797,7 +2794,7 @@
         <v>62</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2806,7 +2803,7 @@
         <v>63</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" ref="J66:J129" si="2">_xlfn.TEXTJOIN($J$1,TRUE,B66:H66)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2815,7 +2812,7 @@
         <v>64</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2824,7 +2821,7 @@
         <v>65</v>
       </c>
       <c r="J68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2833,7 +2830,7 @@
         <v>66</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J69:J132" si="1">_xlfn.TEXTJOIN($J$1,TRUE,$B69:$H69)</f>
         <v/>
       </c>
     </row>
@@ -2842,7 +2839,7 @@
         <v>67</v>
       </c>
       <c r="J70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2851,7 +2848,7 @@
         <v>68</v>
       </c>
       <c r="J71" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2860,7 +2857,7 @@
         <v>69</v>
       </c>
       <c r="J72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2869,7 +2866,7 @@
         <v>70</v>
       </c>
       <c r="J73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2878,7 +2875,7 @@
         <v>71</v>
       </c>
       <c r="J74" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2887,7 +2884,7 @@
         <v>72</v>
       </c>
       <c r="J75" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2896,7 +2893,7 @@
         <v>73</v>
       </c>
       <c r="J76" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2905,7 +2902,7 @@
         <v>74</v>
       </c>
       <c r="J77" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2914,7 +2911,7 @@
         <v>75</v>
       </c>
       <c r="J78" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2923,7 +2920,7 @@
         <v>76</v>
       </c>
       <c r="J79" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2932,7 +2929,7 @@
         <v>77</v>
       </c>
       <c r="J80" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2941,7 +2938,7 @@
         <v>78</v>
       </c>
       <c r="J81" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2950,7 +2947,7 @@
         <v>79</v>
       </c>
       <c r="J82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2959,7 +2956,7 @@
         <v>80</v>
       </c>
       <c r="J83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2968,7 +2965,7 @@
         <v>81</v>
       </c>
       <c r="J84" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2977,7 +2974,7 @@
         <v>82</v>
       </c>
       <c r="J85" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2986,7 +2983,7 @@
         <v>83</v>
       </c>
       <c r="J86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2995,7 +2992,7 @@
         <v>84</v>
       </c>
       <c r="J87" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3004,7 +3001,7 @@
         <v>85</v>
       </c>
       <c r="J88" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3013,7 +3010,7 @@
         <v>86</v>
       </c>
       <c r="J89" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3022,7 +3019,7 @@
         <v>87</v>
       </c>
       <c r="J90" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3031,7 +3028,7 @@
         <v>88</v>
       </c>
       <c r="J91" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3040,7 +3037,7 @@
         <v>89</v>
       </c>
       <c r="J92" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3049,7 +3046,7 @@
         <v>90</v>
       </c>
       <c r="J93" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3058,7 +3055,7 @@
         <v>91</v>
       </c>
       <c r="J94" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3067,7 +3064,7 @@
         <v>92</v>
       </c>
       <c r="J95" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3076,7 +3073,7 @@
         <v>93</v>
       </c>
       <c r="J96" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3085,7 +3082,7 @@
         <v>94</v>
       </c>
       <c r="J97" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3094,7 +3091,7 @@
         <v>95</v>
       </c>
       <c r="J98" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3103,7 +3100,7 @@
         <v>96</v>
       </c>
       <c r="J99" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3112,7 +3109,7 @@
         <v>97</v>
       </c>
       <c r="J100" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3121,7 +3118,7 @@
         <v>98</v>
       </c>
       <c r="J101" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3130,7 +3127,7 @@
         <v>99</v>
       </c>
       <c r="J102" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3139,7 +3136,7 @@
         <v>100</v>
       </c>
       <c r="J103" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3148,7 +3145,7 @@
         <v>101</v>
       </c>
       <c r="J104" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3157,7 +3154,7 @@
         <v>102</v>
       </c>
       <c r="J105" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3166,7 +3163,7 @@
         <v>103</v>
       </c>
       <c r="J106" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3175,7 +3172,7 @@
         <v>104</v>
       </c>
       <c r="J107" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3184,7 +3181,7 @@
         <v>105</v>
       </c>
       <c r="J108" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3193,7 +3190,7 @@
         <v>106</v>
       </c>
       <c r="J109" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3202,7 +3199,7 @@
         <v>107</v>
       </c>
       <c r="J110" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3211,7 +3208,7 @@
         <v>108</v>
       </c>
       <c r="J111" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3220,7 +3217,7 @@
         <v>109</v>
       </c>
       <c r="J112" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3229,7 +3226,7 @@
         <v>110</v>
       </c>
       <c r="J113" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3238,7 +3235,7 @@
         <v>111</v>
       </c>
       <c r="J114" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3247,7 +3244,7 @@
         <v>112</v>
       </c>
       <c r="J115" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3256,7 +3253,7 @@
         <v>113</v>
       </c>
       <c r="J116" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3265,7 +3262,7 @@
         <v>114</v>
       </c>
       <c r="J117" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3274,7 +3271,7 @@
         <v>115</v>
       </c>
       <c r="J118" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3283,7 +3280,7 @@
         <v>116</v>
       </c>
       <c r="J119" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3292,7 +3289,7 @@
         <v>117</v>
       </c>
       <c r="J120" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3301,7 +3298,7 @@
         <v>118</v>
       </c>
       <c r="J121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3310,7 +3307,7 @@
         <v>119</v>
       </c>
       <c r="J122" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3319,7 +3316,7 @@
         <v>120</v>
       </c>
       <c r="J123" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3328,7 +3325,7 @@
         <v>121</v>
       </c>
       <c r="J124" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3337,7 +3334,7 @@
         <v>122</v>
       </c>
       <c r="J125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3346,7 +3343,7 @@
         <v>123</v>
       </c>
       <c r="J126" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3355,7 +3352,7 @@
         <v>124</v>
       </c>
       <c r="J127" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3364,7 +3361,7 @@
         <v>125</v>
       </c>
       <c r="J128" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3373,7 +3370,7 @@
         <v>126</v>
       </c>
       <c r="J129" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3382,7 +3379,7 @@
         <v>127</v>
       </c>
       <c r="J130" t="str">
-        <f t="shared" ref="J130:J193" si="3">_xlfn.TEXTJOIN($J$1,TRUE,B130:H130)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3391,7 +3388,7 @@
         <v>128</v>
       </c>
       <c r="J131" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3400,7 +3397,7 @@
         <v>129</v>
       </c>
       <c r="J132" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3409,7 +3406,7 @@
         <v>130</v>
       </c>
       <c r="J133" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J133:J196" si="2">_xlfn.TEXTJOIN($J$1,TRUE,$B133:$H133)</f>
         <v/>
       </c>
     </row>
@@ -3418,7 +3415,7 @@
         <v>131</v>
       </c>
       <c r="J134" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3427,7 +3424,7 @@
         <v>132</v>
       </c>
       <c r="J135" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3436,7 +3433,7 @@
         <v>133</v>
       </c>
       <c r="J136" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3445,7 +3442,7 @@
         <v>134</v>
       </c>
       <c r="J137" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3454,7 +3451,7 @@
         <v>135</v>
       </c>
       <c r="J138" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3463,7 +3460,7 @@
         <v>136</v>
       </c>
       <c r="J139" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3472,7 +3469,7 @@
         <v>137</v>
       </c>
       <c r="J140" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3481,7 +3478,7 @@
         <v>138</v>
       </c>
       <c r="J141" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3490,7 +3487,7 @@
         <v>139</v>
       </c>
       <c r="J142" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3499,7 +3496,7 @@
         <v>140</v>
       </c>
       <c r="J143" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3508,7 +3505,7 @@
         <v>141</v>
       </c>
       <c r="J144" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3517,7 +3514,7 @@
         <v>142</v>
       </c>
       <c r="J145" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3526,7 +3523,7 @@
         <v>143</v>
       </c>
       <c r="J146" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3535,7 +3532,7 @@
         <v>144</v>
       </c>
       <c r="J147" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3544,7 +3541,7 @@
         <v>145</v>
       </c>
       <c r="J148" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3553,7 +3550,7 @@
         <v>146</v>
       </c>
       <c r="J149" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3562,7 +3559,7 @@
         <v>147</v>
       </c>
       <c r="J150" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3571,7 +3568,7 @@
         <v>148</v>
       </c>
       <c r="J151" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3580,7 +3577,7 @@
         <v>149</v>
       </c>
       <c r="J152" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3589,7 +3586,7 @@
         <v>150</v>
       </c>
       <c r="J153" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3598,7 +3595,7 @@
         <v>151</v>
       </c>
       <c r="J154" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3607,7 +3604,7 @@
         <v>152</v>
       </c>
       <c r="J155" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3616,7 +3613,7 @@
         <v>153</v>
       </c>
       <c r="J156" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3625,7 +3622,7 @@
         <v>154</v>
       </c>
       <c r="J157" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3634,7 +3631,7 @@
         <v>155</v>
       </c>
       <c r="J158" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3643,7 +3640,7 @@
         <v>156</v>
       </c>
       <c r="J159" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3652,7 +3649,7 @@
         <v>157</v>
       </c>
       <c r="J160" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3661,7 +3658,7 @@
         <v>158</v>
       </c>
       <c r="J161" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3670,7 +3667,7 @@
         <v>159</v>
       </c>
       <c r="J162" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3679,7 +3676,7 @@
         <v>160</v>
       </c>
       <c r="J163" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3688,7 +3685,7 @@
         <v>161</v>
       </c>
       <c r="J164" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3697,7 +3694,7 @@
         <v>162</v>
       </c>
       <c r="J165" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3706,7 +3703,7 @@
         <v>163</v>
       </c>
       <c r="J166" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3715,7 +3712,7 @@
         <v>164</v>
       </c>
       <c r="J167" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3724,7 +3721,7 @@
         <v>165</v>
       </c>
       <c r="J168" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3733,7 +3730,7 @@
         <v>166</v>
       </c>
       <c r="J169" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3742,7 +3739,7 @@
         <v>167</v>
       </c>
       <c r="J170" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3751,7 +3748,7 @@
         <v>168</v>
       </c>
       <c r="J171" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3760,7 +3757,7 @@
         <v>169</v>
       </c>
       <c r="J172" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3769,7 +3766,7 @@
         <v>170</v>
       </c>
       <c r="J173" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3778,7 +3775,7 @@
         <v>171</v>
       </c>
       <c r="J174" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3787,7 +3784,7 @@
         <v>172</v>
       </c>
       <c r="J175" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3796,7 +3793,7 @@
         <v>173</v>
       </c>
       <c r="J176" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3805,7 +3802,7 @@
         <v>174</v>
       </c>
       <c r="J177" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3814,7 +3811,7 @@
         <v>175</v>
       </c>
       <c r="J178" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3823,7 +3820,7 @@
         <v>176</v>
       </c>
       <c r="J179" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3832,7 +3829,7 @@
         <v>177</v>
       </c>
       <c r="J180" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3841,7 +3838,7 @@
         <v>178</v>
       </c>
       <c r="J181" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3850,7 +3847,7 @@
         <v>179</v>
       </c>
       <c r="J182" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3859,7 +3856,7 @@
         <v>180</v>
       </c>
       <c r="J183" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3868,7 +3865,7 @@
         <v>181</v>
       </c>
       <c r="J184" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3877,7 +3874,7 @@
         <v>182</v>
       </c>
       <c r="J185" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3886,7 +3883,7 @@
         <v>183</v>
       </c>
       <c r="J186" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3895,7 +3892,7 @@
         <v>184</v>
       </c>
       <c r="J187" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3904,7 +3901,7 @@
         <v>185</v>
       </c>
       <c r="J188" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3913,7 +3910,7 @@
         <v>186</v>
       </c>
       <c r="J189" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3922,7 +3919,7 @@
         <v>187</v>
       </c>
       <c r="J190" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3931,7 +3928,7 @@
         <v>188</v>
       </c>
       <c r="J191" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3940,7 +3937,7 @@
         <v>189</v>
       </c>
       <c r="J192" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3949,7 +3946,7 @@
         <v>190</v>
       </c>
       <c r="J193" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3958,7 +3955,7 @@
         <v>191</v>
       </c>
       <c r="J194" t="str">
-        <f t="shared" ref="J194:J257" si="4">_xlfn.TEXTJOIN($J$1,TRUE,B194:H194)</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3967,7 +3964,7 @@
         <v>192</v>
       </c>
       <c r="J195" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3976,7 +3973,7 @@
         <v>193</v>
       </c>
       <c r="J196" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -3985,7 +3982,7 @@
         <v>194</v>
       </c>
       <c r="J197" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J197:J248" si="3">_xlfn.TEXTJOIN($J$1,TRUE,$B197:$H197)</f>
         <v/>
       </c>
     </row>
@@ -3994,7 +3991,7 @@
         <v>195</v>
       </c>
       <c r="J198" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4003,7 +4000,7 @@
         <v>196</v>
       </c>
       <c r="J199" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4012,7 +4009,7 @@
         <v>197</v>
       </c>
       <c r="J200" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4021,7 +4018,7 @@
         <v>198</v>
       </c>
       <c r="J201" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4030,7 +4027,7 @@
         <v>199</v>
       </c>
       <c r="J202" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4039,7 +4036,7 @@
         <v>200</v>
       </c>
       <c r="J203" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4048,7 +4045,7 @@
         <v>201</v>
       </c>
       <c r="J204" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4057,7 +4054,7 @@
         <v>202</v>
       </c>
       <c r="J205" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4066,7 +4063,7 @@
         <v>203</v>
       </c>
       <c r="J206" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4075,7 +4072,7 @@
         <v>204</v>
       </c>
       <c r="J207" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4084,7 +4081,7 @@
         <v>205</v>
       </c>
       <c r="J208" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4093,7 +4090,7 @@
         <v>206</v>
       </c>
       <c r="J209" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4102,7 +4099,7 @@
         <v>207</v>
       </c>
       <c r="J210" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4111,7 +4108,7 @@
         <v>208</v>
       </c>
       <c r="J211" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4120,7 +4117,7 @@
         <v>209</v>
       </c>
       <c r="J212" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4129,7 +4126,7 @@
         <v>210</v>
       </c>
       <c r="J213" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4138,7 +4135,7 @@
         <v>211</v>
       </c>
       <c r="J214" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4147,7 +4144,7 @@
         <v>212</v>
       </c>
       <c r="J215" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4156,7 +4153,7 @@
         <v>213</v>
       </c>
       <c r="J216" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4165,7 +4162,7 @@
         <v>214</v>
       </c>
       <c r="J217" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4174,7 +4171,7 @@
         <v>215</v>
       </c>
       <c r="J218" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4183,7 +4180,7 @@
         <v>216</v>
       </c>
       <c r="J219" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4192,7 +4189,7 @@
         <v>217</v>
       </c>
       <c r="J220" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4201,7 +4198,7 @@
         <v>218</v>
       </c>
       <c r="J221" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4210,7 +4207,7 @@
         <v>219</v>
       </c>
       <c r="J222" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4219,7 +4216,7 @@
         <v>220</v>
       </c>
       <c r="J223" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4228,7 +4225,7 @@
         <v>221</v>
       </c>
       <c r="J224" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4237,7 +4234,7 @@
         <v>222</v>
       </c>
       <c r="J225" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4246,7 +4243,7 @@
         <v>223</v>
       </c>
       <c r="J226" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4255,7 +4252,7 @@
         <v>224</v>
       </c>
       <c r="J227" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4264,7 +4261,7 @@
         <v>225</v>
       </c>
       <c r="J228" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4273,7 +4270,7 @@
         <v>226</v>
       </c>
       <c r="J229" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4282,7 +4279,7 @@
         <v>227</v>
       </c>
       <c r="J230" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4291,7 +4288,7 @@
         <v>228</v>
       </c>
       <c r="J231" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4300,7 +4297,7 @@
         <v>229</v>
       </c>
       <c r="J232" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4309,7 +4306,7 @@
         <v>230</v>
       </c>
       <c r="J233" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4318,7 +4315,7 @@
         <v>231</v>
       </c>
       <c r="J234" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4327,7 +4324,7 @@
         <v>232</v>
       </c>
       <c r="J235" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4336,7 +4333,7 @@
         <v>233</v>
       </c>
       <c r="J236" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4345,7 +4342,7 @@
         <v>234</v>
       </c>
       <c r="J237" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4354,7 +4351,7 @@
         <v>235</v>
       </c>
       <c r="J238" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4363,7 +4360,7 @@
         <v>236</v>
       </c>
       <c r="J239" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4372,7 +4369,7 @@
         <v>237</v>
       </c>
       <c r="J240" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4381,7 +4378,7 @@
         <v>238</v>
       </c>
       <c r="J241" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4390,7 +4387,7 @@
         <v>239</v>
       </c>
       <c r="J242" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4399,7 +4396,7 @@
         <v>240</v>
       </c>
       <c r="J243" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4408,7 +4405,7 @@
         <v>241</v>
       </c>
       <c r="J244" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4417,7 +4414,7 @@
         <v>242</v>
       </c>
       <c r="J245" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4426,7 +4423,7 @@
         <v>243</v>
       </c>
       <c r="J246" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4435,7 +4432,7 @@
         <v>244</v>
       </c>
       <c r="J247" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -4444,13 +4441,13 @@
         <v>245</v>
       </c>
       <c r="J248" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J249" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J194:J257" si="4">_xlfn.TEXTJOIN($J$1,TRUE,B249:H249)</f>
         <v/>
       </c>
     </row>
@@ -8945,7 +8942,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="J6 J7:J997" formulaRange="1"/>
+    <ignoredError sqref="J249:J997" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -8955,7 +8952,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8969,10 +8966,11 @@
     <row r="1" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="16" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C1" s="17">
-        <v>22425.292969999999</v>
+        <f>SUM(O11:O410)</f>
+        <v>600.9697914123534</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -9000,10 +8998,11 @@
     <row r="2" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="16" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C2" s="18">
-        <v>11.1328125</v>
+        <f>SUM(L11:L410)/1024</f>
+        <v>0.3537778501157407</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -9031,14 +9030,15 @@
     <row r="3" spans="1:25" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="16" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C3" s="18">
-        <v>11.1328125</v>
+        <f>SUM(M11:M410)/1024</f>
+        <v>1.7395019531249998</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="35" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F3" s="35"/>
       <c r="G3" s="35"/>
@@ -9064,10 +9064,11 @@
     <row r="4" spans="1:25" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C4" s="18">
-        <v>10</v>
+        <f>SUM(J11:J410)</f>
+        <v>15</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="35"/>
@@ -9095,10 +9096,10 @@
     <row r="5" spans="1:25" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="16" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C5" s="18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="19"/>
@@ -9126,7 +9127,7 @@
     <row r="6" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="16" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C6" s="18">
         <v>5120</v>
@@ -9157,7 +9158,7 @@
     <row r="7" spans="1:25" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C7" s="18">
         <v>15360</v>
@@ -9214,55 +9215,55 @@
     </row>
     <row r="9" spans="1:25" s="30" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I9" s="31" t="s">
         <v>1</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="P9" s="22" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="Q9" s="22" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="R9" s="29"/>
       <c r="S9" s="29"/>
@@ -9306,24 +9307,24 @@
       </c>
       <c r="B11" s="15" t="str">
         <f>'Stage 1'!J4</f>
-        <v>dev.test.test.object.obj2.v1</v>
+        <v>useast.prod.streamdata.ordering.v1</v>
       </c>
       <c r="C11" s="23">
         <v>0.3</v>
       </c>
       <c r="D11" s="2">
-        <f>1024</f>
-        <v>1024</v>
+        <f>10*1024</f>
+        <v>10240</v>
       </c>
       <c r="E11" s="2">
-        <v>500</v>
+        <f>100000/24/60/60</f>
+        <v>1.1574074074074074</v>
       </c>
       <c r="F11" s="2">
-        <f>7*24</f>
-        <v>168</v>
+        <v>1</v>
       </c>
       <c r="G11" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H11" s="2">
         <v>3</v>
@@ -9333,34 +9334,34 @@
       </c>
       <c r="J11" s="24">
         <f>IFERROR(MAX($C$5, _xlfn.CEILING.MATH(L11/$C$6,1), _xlfn.CEILING.MATH(M11/$C$7,1), _xlfn.CEILING.MATH(N11,1)), 0 )</f>
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="K11" s="25">
         <f t="shared" ref="K11:K74" si="0">(D11*E11)/1024</f>
-        <v>500</v>
+        <v>11.574074074074074</v>
       </c>
       <c r="L11" s="25">
         <f t="shared" ref="L11:L74" si="1">K11+(C11*K11)</f>
-        <v>650</v>
+        <v>15.046296296296298</v>
       </c>
       <c r="M11" s="25">
         <f t="shared" ref="M11:M74" si="2">H11*L11</f>
-        <v>1950</v>
+        <v>45.138888888888893</v>
       </c>
       <c r="N11" s="25">
         <f t="shared" ref="N11:N74" si="3">IFERROR(_xlfn.CEILING.MATH(E11/G11,1), "" )</f>
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="O11" s="25">
         <f t="shared" ref="O11:O74" si="4">((L11*F11*60*60)/1024/1024)*I11</f>
-        <v>1124.725341796875</v>
+        <v>0.15497207641601562</v>
       </c>
       <c r="P11" s="26">
         <v>0.2</v>
       </c>
       <c r="Q11" s="25">
         <f>O11-(P11*O11)</f>
-        <v>899.7802734375</v>
+        <v>0.1239776611328125</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
@@ -9377,61 +9378,62 @@
       </c>
       <c r="B12" s="15" t="str">
         <f>'Stage 1'!J5</f>
-        <v>uat.test.test3.dataplane.datanode.v1</v>
+        <v>uswest.soak.streamdata.oredering.v1</v>
       </c>
       <c r="C12" s="23">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="D12" s="2">
-        <f>55*1024</f>
-        <v>56320</v>
+        <f>2*1024</f>
+        <v>2048</v>
       </c>
       <c r="E12" s="2">
-        <v>250</v>
+        <f>10000000/24/60/60</f>
+        <v>115.74074074074073</v>
       </c>
       <c r="F12" s="2">
-        <f>30*24</f>
-        <v>720</v>
+        <f>7*24</f>
+        <v>168</v>
       </c>
       <c r="G12" s="2">
+        <v>10</v>
+      </c>
+      <c r="H12" s="2">
         <v>5</v>
       </c>
-      <c r="H12" s="2">
-        <v>20</v>
-      </c>
       <c r="I12" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J12" s="24">
         <f t="shared" ref="J12:J75" si="5">IFERROR(MAX($C$5, _xlfn.CEILING.MATH(L12/$C$6,1), _xlfn.CEILING.MATH(M12/$C$7,1), _xlfn.CEILING.MATH(N12,1)), 0 )</f>
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="K12" s="25">
         <f t="shared" si="0"/>
-        <v>13750</v>
+        <v>231.48148148148147</v>
       </c>
       <c r="L12" s="25">
         <f t="shared" si="1"/>
-        <v>22000</v>
+        <v>347.22222222222217</v>
       </c>
       <c r="M12" s="25">
         <f t="shared" si="2"/>
-        <v>440000</v>
+        <v>1736.1111111111109</v>
       </c>
       <c r="N12" s="25">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="O12" s="25">
         <f t="shared" si="4"/>
-        <v>271911.62109375</v>
+        <v>600.81481933593739</v>
       </c>
       <c r="P12" s="26">
         <v>0.2</v>
       </c>
       <c r="Q12" s="25">
         <f t="shared" ref="Q12:Q75" si="6">O12-(P12*O12)</f>
-        <v>217529.296875</v>
+        <v>480.65185546874989</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -30528,11 +30530,11 @@
         <v>0</v>
       </c>
       <c r="L395" s="25">
-        <f t="shared" ref="L395:L458" si="43">K395+(C395*K395)</f>
+        <f t="shared" ref="L395:L410" si="43">K395+(C395*K395)</f>
         <v>0</v>
       </c>
       <c r="M395" s="25">
-        <f t="shared" ref="M395:M458" si="44">H395*L395</f>
+        <f t="shared" ref="M395:M410" si="44">H395*L395</f>
         <v>0</v>
       </c>
       <c r="N395" s="25" t="str">
@@ -47327,7 +47329,7 @@
   <dimension ref="A2:OL41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -47353,84 +47355,84 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
-      <c r="O3" s="71" t="s">
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="69"/>
+      <c r="O3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="73"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="42"/>
     </row>
     <row r="4" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="64"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="75"/>
-      <c r="Q4" s="76"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
+      <c r="M4" s="72"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="45"/>
     </row>
     <row r="5" spans="1:18" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <f>MAX(B6:L6)</f>
-        <v>14</v>
-      </c>
-      <c r="B5" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="37" t="s">
+      <c r="C5" s="49"/>
+      <c r="D5" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="37" t="s">
+      <c r="E5" s="49"/>
+      <c r="F5" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="37" t="s">
+      <c r="G5" s="49"/>
+      <c r="H5" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="37" t="s">
+      <c r="I5" s="49"/>
+      <c r="J5" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="37" t="s">
+      <c r="K5" s="49"/>
+      <c r="L5" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="38"/>
+      <c r="M5" s="49"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="69" t="s">
+      <c r="P5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="70"/>
+      <c r="Q5" s="47"/>
     </row>
     <row r="6" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="str" cm="1">
+      <c r="A6" s="62" t="str" cm="1">
         <f t="array" ref="A6">_xlfn.SWITCH(A5,B6," The Cluster is bound by Average Ingress Network data and considered as minimum, considering Network Ingress throttling for as potential bottleneck for Average data ingress",
 D6," The cluster is limited by Average total bandwidth available for the cluster. Please use the recommended number of brokers to cater well to both Producers and Consumers without bandwidth issues.",
 F6," The cluster is Ingress Disk write bound and the inbound data is more than what the cluster as a whole can handle. Please consider upgrading Disk Write throughput or using the recommended number of brokers",
@@ -47439,96 +47441,96 @@
 L6," The broker count is limited at the soft limit for replica count per broker node. This is as per recommendations from Jun Rao in his blogs. Please modify cell G11 to taste.")</f>
         <v xml:space="preserve"> The cluster is disk capacity bound and data retention policy needs either more brokers with equal capacity disks or more disk capacity is needed. This considers equal data distribution across the cluster.</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="52">
         <f>CEILING((L10/D13)/D15,1)</f>
         <v>1</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="39">
+      <c r="C6" s="53"/>
+      <c r="D6" s="52">
         <f>CEILING(((L12+L10)/(D13+D14))/D15, 1)</f>
         <v>1</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="39">
+      <c r="E6" s="53"/>
+      <c r="F6" s="52">
         <f>CEILING(((L10+L15)/D11),1)</f>
         <v>1</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="39">
+      <c r="G6" s="53"/>
+      <c r="H6" s="52">
         <f>CEILING(L14/D10,1)</f>
-        <v>14</v>
-      </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="39">
+        <v>7</v>
+      </c>
+      <c r="I6" s="53"/>
+      <c r="J6" s="52">
         <f>CEILING(B20,1)</f>
-        <v>5</v>
-      </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="65">
+        <v>3</v>
+      </c>
+      <c r="K6" s="53"/>
+      <c r="L6" s="73">
         <f>CEILING(G12/G10,1)</f>
         <v>1</v>
       </c>
-      <c r="M6" s="66"/>
+      <c r="M6" s="74"/>
       <c r="O6" s="6"/>
-      <c r="P6" s="69" t="s">
+      <c r="P6" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="70"/>
+      <c r="Q6" s="47"/>
     </row>
     <row r="7" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="68"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="76"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="69" t="s">
+      <c r="P7" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" s="70"/>
+      <c r="Q7" s="47"/>
     </row>
     <row r="8" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="55"/>
-      <c r="B8" s="48" t="s">
+      <c r="A8" s="63"/>
+      <c r="B8" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="57" t="s">
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="43" t="s">
+      <c r="F8" s="56"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
       <c r="R8" s="13"/>
     </row>
     <row r="9" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="55"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
       <c r="N9" s="36" t="s">
         <v>48</v>
       </c>
@@ -47537,23 +47539,23 @@
       <c r="Q9" s="36"/>
       <c r="R9" s="4">
         <f>CEILING(B38/L6,1)</f>
-        <v>75</v>
+        <v>390</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="45" t="s">
+      <c r="A10" s="64"/>
+      <c r="B10" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="9">
-        <f>1024*16</f>
-        <v>16384</v>
-      </c>
-      <c r="E10" s="47" t="s">
+        <f>2*1024</f>
+        <v>2048</v>
+      </c>
+      <c r="E10" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="46"/>
+      <c r="F10" s="51"/>
       <c r="G10" s="11">
         <v>4500</v>
       </c>
@@ -47566,7 +47568,7 @@
       <c r="K10" s="36"/>
       <c r="L10" s="4">
         <f t="shared" ref="L10:L15" si="1">B31</f>
-        <v>13.92</v>
+        <v>5.09</v>
       </c>
       <c r="N10" s="36" t="s">
         <v>49</v>
@@ -47576,21 +47578,21 @@
       <c r="Q10" s="36"/>
       <c r="R10" s="4">
         <f>CEILING(G13-R9, 1)</f>
-        <v>-51</v>
+        <v>-222</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="9">
-        <v>350</v>
-      </c>
-      <c r="E11" s="47" t="s">
+        <v>500</v>
+      </c>
+      <c r="E11" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="46"/>
+      <c r="F11" s="51"/>
       <c r="G11" s="11">
         <v>100000</v>
       </c>
@@ -47603,35 +47605,35 @@
       <c r="K11" s="36"/>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>13.92</v>
-      </c>
-      <c r="N11" s="77" t="s">
+        <v>5.09</v>
+      </c>
+      <c r="N11" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="O11" s="78"/>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="79"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="39"/>
       <c r="R11" s="4">
         <f>R14+1024</f>
-        <v>2817024</v>
+        <v>513024</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="E12" s="47" t="str">
+        <v>0.65</v>
+      </c>
+      <c r="E12" s="50" t="str">
         <f>A37</f>
         <v>Total Partition Count Incl. Replicas</v>
       </c>
-      <c r="F12" s="46"/>
+      <c r="F12" s="51"/>
       <c r="G12" s="4">
         <f>$B$37</f>
-        <v>325</v>
+        <v>1170</v>
       </c>
       <c r="H12" s="36" t="str">
         <f t="shared" si="0"/>
@@ -47642,35 +47644,35 @@
       <c r="K12" s="36"/>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>270.02</v>
-      </c>
-      <c r="N12" s="77" t="s">
+        <v>24.310000000000002</v>
+      </c>
+      <c r="N12" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="78"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="79"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="39"/>
       <c r="R12" s="4">
         <f>MAX(C24:INDEX(24:24,COLUMNS(24:24)))+1024</f>
-        <v>57344</v>
+        <v>11264</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="9">
         <f>((10*1024)/2)/8</f>
         <v>640</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="46"/>
+      <c r="F13" s="51"/>
       <c r="G13" s="4">
         <f>CEILING(G12/A5,1)</f>
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="H13" s="36" t="str">
         <f t="shared" si="0"/>
@@ -47681,19 +47683,19 @@
       <c r="K13" s="36"/>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>270.02</v>
-      </c>
-      <c r="N13" s="77"/>
-      <c r="O13" s="78"/>
-      <c r="P13" s="78"/>
-      <c r="Q13" s="79"/>
+        <v>24.310000000000002</v>
+      </c>
+      <c r="N13" s="37"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="39"/>
       <c r="R13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="9">
         <f>((10*1024)/2)/8</f>
         <v>640</v>
@@ -47707,7 +47709,7 @@
       <c r="K14" s="36"/>
       <c r="L14" s="4">
         <f t="shared" si="1"/>
-        <v>213512.43</v>
+        <v>12333.58</v>
       </c>
       <c r="N14" s="36" t="s">
         <v>29</v>
@@ -47719,16 +47721,16 @@
       </c>
       <c r="R14" s="4">
         <f>(MAX(C22:INDEX(22:22,COLUMNS(22:22)))*Q14)</f>
-        <v>2816000</v>
+        <v>512000</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="46"/>
+      <c r="C15" s="51"/>
       <c r="D15" s="10">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="H15" s="36" t="str">
         <f t="shared" si="0"/>
@@ -47739,7 +47741,7 @@
       <c r="K15" s="36"/>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
-        <v>54.69</v>
+        <v>10.18</v>
       </c>
       <c r="N15" s="36" t="s">
         <v>30</v>
@@ -47763,7 +47765,7 @@
       <c r="K16" s="36"/>
       <c r="L16" s="4">
         <f>L14/A5</f>
-        <v>15250.887857142856</v>
+        <v>1761.94</v>
       </c>
     </row>
     <row r="18" spans="1:402" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -47775,10 +47777,10 @@
       </c>
       <c r="C18" s="34" t="str" cm="1">
         <f t="array" ref="C18:OL18">TRANSPOSE('Stage 2'!$B$11:B410)</f>
-        <v>dev.test.test.object.obj2.v1</v>
+        <v>useast.prod.streamdata.ordering.v1</v>
       </c>
       <c r="D18" s="34" t="str">
-        <v>uat.test.test3.dataplane.datanode.v1</v>
+        <v>uswest.soak.streamdata.oredering.v1</v>
       </c>
       <c r="E18" s="34" t="str">
         <v/>
@@ -48981,14 +48983,14 @@
       </c>
       <c r="B19" s="8">
         <f>SUM(C19:INDEX(19:19,COLUMNS(19:19)))</f>
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="C19" cm="1">
         <f t="array" ref="C19:OL19">TRANSPOSE('Stage 2'!$J$11:J410)</f>
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -50191,14 +50193,14 @@
       </c>
       <c r="B20" s="8">
         <f>MAX(C20:AZ20)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C20" cm="1">
         <f t="array" ref="C20:OL20">TRANSPOSE('Stage 2'!$I$11:I410)</f>
         <v>3</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -51402,10 +51404,10 @@
       <c r="B21" s="8"/>
       <c r="C21" cm="1">
         <f t="array" ref="C21:OL21">TRANSPOSE('Stage 2'!$F$11:F410)</f>
+        <v>1</v>
+      </c>
+      <c r="D21">
         <v>168</v>
-      </c>
-      <c r="D21">
-        <v>720</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -52608,14 +52610,14 @@
       </c>
       <c r="B22" s="8">
         <f>SUM(C22:INDEX(22:22,COLUMNS(22:22)))</f>
-        <v>57344</v>
+        <v>12288</v>
       </c>
       <c r="C22" cm="1">
         <f t="array" ref="C22:OL22">TRANSPOSE('Stage 2'!$D$11:D410)</f>
-        <v>1024</v>
+        <v>10240</v>
       </c>
       <c r="D22">
-        <v>56320</v>
+        <v>2048</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -53818,14 +53820,14 @@
       </c>
       <c r="B23" s="8">
         <f>SUM(C23:INDEX(23:23,COLUMNS(23:23)))</f>
-        <v>750</v>
+        <v>116.89814814814814</v>
       </c>
       <c r="C23" cm="1">
         <f t="array" ref="C23:OL23">TRANSPOSE('Stage 2'!$E$11:E410)</f>
-        <v>500</v>
+        <v>1.1574074074074074</v>
       </c>
       <c r="D23">
-        <v>250</v>
+        <v>115.74074074074073</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -55028,14 +55030,14 @@
       </c>
       <c r="B24" s="8">
         <f>SUM(C24:INDEX(24:24,COLUMNS(24:24)))</f>
-        <v>57344</v>
+        <v>12288</v>
       </c>
       <c r="C24" cm="1">
         <f t="array" ref="C24:OL24">TRANSPOSE('Stage 2'!$D$11:D410)</f>
-        <v>1024</v>
+        <v>10240</v>
       </c>
       <c r="D24">
-        <v>56320</v>
+        <v>2048</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -56238,14 +56240,14 @@
       </c>
       <c r="B25" s="8">
         <f>SUM(C25:INDEX(25:25,COLUMNS(25:25)))</f>
-        <v>750</v>
+        <v>116.89814814814814</v>
       </c>
       <c r="C25" cm="1">
         <f t="array" ref="C25:OL25">TRANSPOSE('Stage 2'!$E$11:E410)</f>
-        <v>500</v>
+        <v>1.1574074074074074</v>
       </c>
       <c r="D25">
-        <v>250</v>
+        <v>115.74074074074073</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -57452,7 +57454,7 @@
         <v>3</v>
       </c>
       <c r="D26">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -58655,18 +58657,16 @@
       </c>
       <c r="B27" s="8">
         <f>SUM(C27:INDEX(27:27,COLUMNS(27:27)))</f>
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="C27">
-        <f>IF(C18="",0,1)</f>
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:BO27" si="2">IF(D18="",0,1)</f>
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E27">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D27:BO27" si="2">IF(E18="",0,1)</f>
         <v>0</v>
       </c>
       <c r="F27">
@@ -60264,15 +60264,15 @@
       </c>
       <c r="B31" s="3">
         <f>CEILING(SUM(C31:INDEX(31:31,COLUMNS(31:31))),0.01)</f>
-        <v>13.92</v>
+        <v>5.09</v>
       </c>
       <c r="C31">
         <f>((((C22*C23)/1024)/1024)*C27)</f>
-        <v>0.48828125</v>
+        <v>0.56514033564814814</v>
       </c>
       <c r="D31">
         <f t="shared" ref="D31:AZ31" si="9">((((D22*D23)/1024)/1024)*D27)</f>
-        <v>13.427734375</v>
+        <v>4.5211226851851851</v>
       </c>
       <c r="E31">
         <f t="shared" si="9"/>
@@ -61873,15 +61873,15 @@
       </c>
       <c r="B32" s="3">
         <f>CEILING(SUM(C32:INDEX(32:32,COLUMNS(32:32))),0.01)</f>
-        <v>13.92</v>
+        <v>5.09</v>
       </c>
       <c r="C32" s="2">
         <f>((((C24*C25)/1024)/1024)*C27)</f>
-        <v>0.48828125</v>
+        <v>0.56514033564814814</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" ref="D32:AZ32" si="16">((((D24*D25)/1024)/1024)*D27)</f>
-        <v>13.427734375</v>
+        <v>4.5211226851851851</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="16"/>
@@ -63482,15 +63482,15 @@
       </c>
       <c r="B33" s="3">
         <f>CEILING(SUM(C33:INDEX(33:33,COLUMNS(33:33))),0.01)</f>
-        <v>270.02</v>
+        <v>24.310000000000002</v>
       </c>
       <c r="C33">
         <f>C31*C26</f>
-        <v>1.46484375</v>
+        <v>1.6954210069444444</v>
       </c>
       <c r="D33">
         <f t="shared" ref="D33:AZ33" si="23">D31*D26</f>
-        <v>268.5546875</v>
+        <v>22.605613425925924</v>
       </c>
       <c r="E33">
         <f t="shared" si="23"/>
@@ -65091,15 +65091,15 @@
       </c>
       <c r="B34" s="3">
         <f>CEILING(SUM(C34:INDEX(34:34,COLUMNS(34:34))),0.01)</f>
-        <v>270.02</v>
+        <v>24.310000000000002</v>
       </c>
       <c r="C34">
         <f>C32*C26</f>
-        <v>1.46484375</v>
+        <v>1.6954210069444444</v>
       </c>
       <c r="D34">
         <f t="shared" ref="D34:AZ34" si="30">D32*D26</f>
-        <v>268.5546875</v>
+        <v>22.605613425925924</v>
       </c>
       <c r="E34">
         <f t="shared" si="30"/>
@@ -66700,15 +66700,15 @@
       </c>
       <c r="B35" s="3">
         <f>CEILING((SUM(C35:INDEX(35:35,COLUMNS(35:35))))/D12,0.01)</f>
-        <v>213512.43</v>
+        <v>12333.58</v>
       </c>
       <c r="C35">
         <f>((C31*C21*60*60*C20)/1024)</f>
-        <v>865.17333984375</v>
+        <v>5.9604644775390616</v>
       </c>
       <c r="D35">
         <f t="shared" ref="D35:AZ35" si="37">((D31*D21*60*60*D20)/1024)</f>
-        <v>169944.76318359375</v>
+        <v>8010.8642578125</v>
       </c>
       <c r="E35">
         <f t="shared" si="37"/>
@@ -68309,15 +68309,15 @@
       </c>
       <c r="B36" s="3">
         <f>CEILING(SUM(C36:INDEX(36:36,COLUMNS(36:36))),0.01)</f>
-        <v>54.69</v>
+        <v>10.18</v>
       </c>
       <c r="C36">
         <f>C31*(C20-1)</f>
-        <v>0.9765625</v>
+        <v>1.1302806712962963</v>
       </c>
       <c r="D36">
         <f t="shared" ref="D36:AZ36" si="44">D31*(D20-1)</f>
-        <v>53.7109375</v>
+        <v>9.0422453703703702</v>
       </c>
       <c r="E36">
         <f t="shared" si="44"/>
@@ -69918,15 +69918,15 @@
       </c>
       <c r="B37" s="3">
         <f>CEILING(SUM(C37:INDEX(37:37,COLUMNS(37:37))),0.01)</f>
-        <v>325</v>
+        <v>1170</v>
       </c>
       <c r="C37">
         <f>C27*C19*C20</f>
-        <v>75</v>
+        <v>450</v>
       </c>
       <c r="D37">
         <f t="shared" ref="D37:AZ37" si="51">D27*D19*D20</f>
-        <v>250</v>
+        <v>720</v>
       </c>
       <c r="E37">
         <f t="shared" si="51"/>
@@ -71527,15 +71527,15 @@
       </c>
       <c r="B38" s="3">
         <f>CEILING(SUM(C38:INDEX(38:38,COLUMNS(38:38))),0.01)</f>
-        <v>75</v>
+        <v>390</v>
       </c>
       <c r="C38">
         <f>C19*C27</f>
-        <v>25</v>
+        <v>150</v>
       </c>
       <c r="D38">
         <f t="shared" ref="D38:AZ38" si="58">D19*D27</f>
-        <v>50</v>
+        <v>240</v>
       </c>
       <c r="E38">
         <f t="shared" si="58"/>
@@ -73133,20 +73133,22 @@
     <row r="41" spans="1:402" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="O3:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H8:L9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="F6:G7"/>
     <mergeCell ref="J6:K7"/>
@@ -73163,22 +73165,20 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H8:L9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="O3:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="N14:P14"/>
   </mergeCells>
   <conditionalFormatting sqref="G12">
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="greaterThan">

</xml_diff>